<commit_message>
Updated docs with new generated files
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-followup-extension.xlsx
+++ b/docs/StructureDefinition-followup-extension.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-05-05T10:23:37+02:00</t>
+    <t>2025-05-11T16:39:14+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -129,7 +129,7 @@
     <t>Context</t>
   </si>
   <si>
-    <t>element:MedicationRequest</t>
+    <t>element:http://example.org/StructureDefinition/my-medicationrequest#MedicationRequest</t>
   </si>
   <si>
     <t>ID</t>

</xml_diff>